<commit_message>
General update of progress
Found mistake in reduced mass term and corrected it. Further developed analysis of comparison of azure reaction rate calculation and my own.
</commit_message>
<xml_diff>
--- a/TESTING/legendre_out/DATA/p0/a0/p0_rates.xlsx
+++ b/TESTING/legendre_out/DATA/p0/a0/p0_rates.xlsx
@@ -595,7 +595,7 @@
         <v>0.03</v>
       </c>
       <c r="C21" t="n">
-        <v>1.069925572247426e-293</v>
+        <v>5.77690575018865e-294</v>
       </c>
     </row>
     <row r="22">
@@ -606,7 +606,7 @@
         <v>0.04</v>
       </c>
       <c r="C22" t="n">
-        <v>1.618396017392157e-223</v>
+        <v>8.73829380307184e-224</v>
       </c>
     </row>
     <row r="23">
@@ -617,7 +617,7 @@
         <v>0.05</v>
       </c>
       <c r="C23" t="n">
-        <v>4.531762361298315e-181</v>
+        <v>2.446858791308649e-181</v>
       </c>
     </row>
     <row r="24">
@@ -628,7 +628,7 @@
         <v>0.06</v>
       </c>
       <c r="C24" t="n">
-        <v>1.464073101292507e-152</v>
+        <v>7.905047162642377e-153</v>
       </c>
     </row>
     <row r="25">
@@ -639,7 +639,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>4.706398329390646e-132</v>
+        <v>2.541150349171852e-132</v>
       </c>
     </row>
     <row r="26">
@@ -650,7 +650,7 @@
         <v>0.08</v>
       </c>
       <c r="C26" t="n">
-        <v>1.433321047415678e-116</v>
+        <v>7.739005551381953e-117</v>
       </c>
     </row>
     <row r="27">
@@ -661,7 +661,7 @@
         <v>0.09</v>
       </c>
       <c r="C27" t="n">
-        <v>1.892244190281698e-104</v>
+        <v>1.02168934875685e-104</v>
       </c>
     </row>
     <row r="28">
@@ -672,7 +672,7 @@
         <v>0.1</v>
       </c>
       <c r="C28" t="n">
-        <v>1.081587264716401e-94</v>
+        <v>5.839870991935935e-95</v>
       </c>
     </row>
     <row r="29">
@@ -683,7 +683,7 @@
         <v>0.11</v>
       </c>
       <c r="C29" t="n">
-        <v>1.163011175861193e-86</v>
+        <v>6.279507388237319e-87</v>
       </c>
     </row>
     <row r="30">
@@ -694,7 +694,7 @@
         <v>0.12</v>
       </c>
       <c r="C30" t="n">
-        <v>6.282515070670159e-80</v>
+        <v>3.392151373416583e-80</v>
       </c>
     </row>
     <row r="31">
@@ -705,7 +705,7 @@
         <v>0.13</v>
       </c>
       <c r="C31" t="n">
-        <v>3.372023492264388e-74</v>
+        <v>1.820674350880554e-74</v>
       </c>
     </row>
     <row r="32">
@@ -716,7 +716,7 @@
         <v>0.14</v>
       </c>
       <c r="C32" t="n">
-        <v>2.930899105540622e-69</v>
+        <v>1.582495736526903e-69</v>
       </c>
     </row>
     <row r="33">
@@ -727,7 +727,7 @@
         <v>0.15</v>
       </c>
       <c r="C33" t="n">
-        <v>5.908235480352249e-65</v>
+        <v>3.190064581093582e-65</v>
       </c>
     </row>
     <row r="34">
@@ -738,7 +738,7 @@
         <v>0.16</v>
       </c>
       <c r="C34" t="n">
-        <v>3.618791457168111e-61</v>
+        <v>1.953913053992746e-61</v>
       </c>
     </row>
     <row r="35">
@@ -749,7 +749,7 @@
         <v>0.18</v>
       </c>
       <c r="C35" t="n">
-        <v>8.329864696049586e-55</v>
+        <v>4.497587531792497e-55</v>
       </c>
     </row>
     <row r="36">
@@ -760,7 +760,7 @@
         <v>0.2</v>
       </c>
       <c r="C36" t="n">
-        <v>1.160149259043231e-49</v>
+        <v>6.264054735439408e-50</v>
       </c>
     </row>
     <row r="37">
@@ -771,7 +771,7 @@
         <v>0.25</v>
       </c>
       <c r="C37" t="n">
-        <v>3.066477520062269e-40</v>
+        <v>1.655699656302115e-40</v>
       </c>
     </row>
     <row r="38">
@@ -782,7 +782,7 @@
         <v>0.3</v>
       </c>
       <c r="C38" t="n">
-        <v>1.048624630541821e-33</v>
+        <v>5.661966877745586e-34</v>
       </c>
     </row>
     <row r="39">
@@ -793,7 +793,7 @@
         <v>0.35</v>
       </c>
       <c r="C39" t="n">
-        <v>2.075692479972294e-28</v>
+        <v>1.120799781879818e-28</v>
       </c>
     </row>
     <row r="40">
@@ -804,7 +804,7 @@
         <v>0.4</v>
       </c>
       <c r="C40" t="n">
-        <v>4.480137291358568e-24</v>
+        <v>2.419149930997881e-24</v>
       </c>
     </row>
     <row r="41">
@@ -815,7 +815,7 @@
         <v>0.45</v>
       </c>
       <c r="C41" t="n">
-        <v>1.167313773422018e-20</v>
+        <v>6.303221746413665e-21</v>
       </c>
     </row>
     <row r="42">
@@ -826,7 +826,7 @@
         <v>0.5</v>
       </c>
       <c r="C42" t="n">
-        <v>6.318072698732577e-18</v>
+        <v>3.411646885679765e-18</v>
       </c>
     </row>
     <row r="43">
@@ -837,7 +837,7 @@
         <v>0.6</v>
       </c>
       <c r="C43" t="n">
-        <v>7.762573475218819e-14</v>
+        <v>4.191793247700701e-14</v>
       </c>
     </row>
     <row r="44">
@@ -848,7 +848,7 @@
         <v>0.7</v>
       </c>
       <c r="C44" t="n">
-        <v>6.299282415337064e-11</v>
+        <v>3.401799724614606e-11</v>
       </c>
     </row>
     <row r="45">
@@ -859,7 +859,7 @@
         <v>0.8</v>
       </c>
       <c r="C45" t="n">
-        <v>9.406290336393287e-09</v>
+        <v>5.080053103998901e-09</v>
       </c>
     </row>
     <row r="46">
@@ -870,7 +870,7 @@
         <v>0.9</v>
       </c>
       <c r="C46" t="n">
-        <v>4.565020251900651e-07</v>
+        <v>2.465654323714587e-07</v>
       </c>
     </row>
     <row r="47">
@@ -881,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>1.012297011335887e-05</v>
+        <v>5.468177354599642e-06</v>
       </c>
     </row>
     <row r="48">
@@ -892,7 +892,7 @@
         <v>1.25</v>
       </c>
       <c r="C48" t="n">
-        <v>0.002654026057010373</v>
+        <v>0.00143404764608668</v>
       </c>
     </row>
     <row r="49">
@@ -903,7 +903,7 @@
         <v>1.5</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1095471509476604</v>
+        <v>0.05920742882708949</v>
       </c>
     </row>
     <row r="50">
@@ -914,7 +914,7 @@
         <v>1.75</v>
       </c>
       <c r="C50" t="n">
-        <v>1.59590128458291</v>
+        <v>0.8627231011645121</v>
       </c>
     </row>
     <row r="51">
@@ -925,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>12.23074142332539</v>
+        <v>6.612629387137179</v>
       </c>
     </row>
     <row r="52">
@@ -936,7 +936,7 @@
         <v>2.5</v>
       </c>
       <c r="C52" t="n">
-        <v>228.4431643461886</v>
+        <v>123.51503246558</v>
       </c>
     </row>
     <row r="53">
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="n">
-        <v>1740.34066261621</v>
+        <v>940.8579914002082</v>
       </c>
     </row>
     <row r="54">
@@ -958,7 +958,7 @@
         <v>3.5</v>
       </c>
       <c r="C54" t="n">
-        <v>7810.563956815336</v>
+        <v>4221.813601361049</v>
       </c>
     </row>
     <row r="55">
@@ -969,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>24797.90624478336</v>
+        <v>13401.75826439215</v>
       </c>
     </row>
     <row r="56">
@@ -980,7 +980,7 @@
         <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>129391.9867976547</v>
+        <v>69911.28735052758</v>
       </c>
     </row>
     <row r="57">
@@ -991,7 +991,7 @@
         <v>6</v>
       </c>
       <c r="C57" t="n">
-        <v>393174.1354147498</v>
+        <v>212400.8247670185</v>
       </c>
     </row>
     <row r="58">
@@ -1002,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="C58" t="n">
-        <v>864473.7899011589</v>
+        <v>466958.7204594503</v>
       </c>
     </row>
     <row r="59">
@@ -1013,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="n">
-        <v>1544332.705186042</v>
+        <v>834136.9215335664</v>
       </c>
     </row>
     <row r="60">
@@ -1024,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="C60" t="n">
-        <v>2397572.629823133</v>
+        <v>1294931.889329147</v>
       </c>
     </row>
     <row r="61">
@@ -1035,7 +1035,7 @@
         <v>10</v>
       </c>
       <c r="C61" t="n">
-        <v>3372053.769518234</v>
+        <v>1821184.720867028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>